<commit_message>
DSA excel sheet by shraddha madam
</commit_message>
<xml_diff>
--- a/DSA by Shradha Ma'am.xlsx
+++ b/DSA by Shradha Ma'am.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RAVIJ PARIKH\Desktop\aditya verma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C06456F-292D-45D3-AA2E-09D7CB00E338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C34B8C34-B105-4CEF-8044-7BF9790DDD75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,10 +24,10 @@
   </definedNames>
   <calcPr calcId="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 1" guid="{271D12BD-D214-4258-BD2A-DFAFD2CDEF5E}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 3" guid="{0C3DE106-6FCF-4530-996A-D1668DB454A5}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 2" guid="{76E63A84-2BB3-4812-AB1F-9EF289858249}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter 4" guid="{51E364FE-A9EC-4DFD-BDF8-1579B81C26CC}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 2" guid="{76E63A84-2BB3-4812-AB1F-9EF289858249}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 3" guid="{0C3DE106-6FCF-4530-996A-D1668DB454A5}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 1" guid="{271D12BD-D214-4258-BD2A-DFAFD2CDEF5E}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -2329,7 +2329,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2396,6 +2396,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor rgb="FFB6D7A8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FFD9EAD3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FFB6D7A8"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -2409,7 +2433,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2533,6 +2557,22 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2755,8 +2795,8 @@
   </sheetPr>
   <dimension ref="A1:Z919"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41:D41"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3174,16 +3214,16 @@
       <c r="Z13" s="2"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="42" t="s">
         <v>21</v>
       </c>
       <c r="E14" s="2"/>
@@ -3278,16 +3318,16 @@
       <c r="Z16" s="2"/>
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="39" t="s">
+      <c r="A17" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="43" t="s">
+      <c r="B17" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="41" t="s">
+      <c r="C17" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="42"/>
+      <c r="D17" s="52"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -3518,16 +3558,16 @@
       <c r="Z23" s="2"/>
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="8" t="s">
+      <c r="A24" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C24" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="D24" s="2"/>
+      <c r="D24" s="42"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
@@ -3552,16 +3592,16 @@
       <c r="Z24" s="2"/>
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="8" t="s">
+      <c r="A25" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C25" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="D25" s="2"/>
+      <c r="D25" s="52"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
@@ -30623,21 +30663,21 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{271D12BD-D214-4258-BD2A-DFAFD2CDEF5E}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{76E63A84-2BB3-4812-AB1F-9EF289858249}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A293:C332" xr:uid="{B3B9CD00-109E-4D72-9027-50D6F252053A}"/>
+      <autoFilter ref="A11:C37" xr:uid="{1611F04C-A76D-4ABC-BB2B-03054CA41092}"/>
+    </customSheetView>
+    <customSheetView guid="{0C3DE106-6FCF-4530-996A-D1668DB454A5}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A11:D37" xr:uid="{31E2BEB3-9A1E-4E6D-BBED-4A128EE3B820}"/>
     </customSheetView>
     <customSheetView guid="{51E364FE-A9EC-4DFD-BDF8-1579B81C26CC}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:D37" xr:uid="{6FFB7E11-4F5D-4D20-9423-93B2ACAA565B}"/>
+      <autoFilter ref="A11:D37" xr:uid="{7ADB44EA-53C8-49B8-95DB-F229AA24227D}"/>
     </customSheetView>
-    <customSheetView guid="{0C3DE106-6FCF-4530-996A-D1668DB454A5}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{271D12BD-D214-4258-BD2A-DFAFD2CDEF5E}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:D37" xr:uid="{3E2916F0-D243-4F50-A41D-E758ED06803A}"/>
-    </customSheetView>
-    <customSheetView guid="{76E63A84-2BB3-4812-AB1F-9EF289858249}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:C37" xr:uid="{C96CCA63-722E-4A7E-99BB-CE8FFFE31FA8}"/>
+      <autoFilter ref="A293:C332" xr:uid="{1C1E5611-602C-4892-A619-2804E9A0ABDF}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="3">

</xml_diff>